<commit_message>
LL-Table(v1.7) - unary minus in print support
</commit_message>
<xml_diff>
--- a/doc/parser/ll_table.xlsx
+++ b/doc/parser/ll_table.xlsx
@@ -21,14 +21,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="188">
-  <si>
-    <t xml:space="preserve">LL Table IFJ17 (v1.6)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="190">
+  <si>
+    <t xml:space="preserve">LL Table IFJ17 (v1.7)</t>
   </si>
   <si>
     <t xml:space="preserve">24/11/2017</t>
   </si>
   <si>
+    <t xml:space="preserve">git q</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keywords</t>
   </si>
   <si>
@@ -159,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">EOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-(SUB)</t>
   </si>
   <si>
     <t xml:space="preserve">=</t>
@@ -1075,10 +1081,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX42"/>
+  <dimension ref="A1:AY42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1125,11 +1131,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="5.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="5.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="43" style="0" width="3.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="7.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="4.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="52" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="44" style="0" width="3.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="7.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="4.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="53" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,9 +1169,14 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1197,12 +1209,12 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL4" s="5"/>
       <c r="AM4" s="5"/>
@@ -1215,163 +1227,167 @@
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
       <c r="AV4" s="5"/>
-      <c r="AW4" s="6"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY5" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX5" s="7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="n">
@@ -1430,16 +1446,17 @@
       <c r="AU6" s="11"/>
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
-      <c r="AX6" s="10" t="s">
-        <v>54</v>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -1489,19 +1506,20 @@
       <c r="AT7" s="15"/>
       <c r="AU7" s="15"/>
       <c r="AV7" s="15"/>
-      <c r="AW7" s="15" t="n">
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="AX7" s="14" t="s">
-        <v>56</v>
+      <c r="AY7" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="n">
@@ -1560,16 +1578,17 @@
       <c r="AU8" s="11"/>
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
-      <c r="AX8" s="10" t="s">
-        <v>58</v>
+      <c r="AX8" s="11"/>
+      <c r="AY8" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1644,16 +1663,17 @@
       <c r="AU9" s="15"/>
       <c r="AV9" s="15"/>
       <c r="AW9" s="15"/>
-      <c r="AX9" s="14" t="s">
-        <v>60</v>
+      <c r="AX9" s="15"/>
+      <c r="AY9" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1738,16 +1758,17 @@
       <c r="AU10" s="11"/>
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
-      <c r="AX10" s="10" t="s">
-        <v>62</v>
+      <c r="AX10" s="11"/>
+      <c r="AY10" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1800,16 +1821,17 @@
       <c r="AU11" s="15"/>
       <c r="AV11" s="15"/>
       <c r="AW11" s="15"/>
-      <c r="AX11" s="14" t="s">
-        <v>64</v>
+      <c r="AX11" s="15"/>
+      <c r="AY11" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1860,16 +1882,17 @@
       <c r="AU12" s="11"/>
       <c r="AV12" s="11"/>
       <c r="AW12" s="11"/>
-      <c r="AX12" s="10" t="s">
-        <v>66</v>
+      <c r="AX12" s="11"/>
+      <c r="AY12" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1920,16 +1943,17 @@
       <c r="AU13" s="15"/>
       <c r="AV13" s="15"/>
       <c r="AW13" s="15"/>
-      <c r="AX13" s="14" t="s">
-        <v>68</v>
+      <c r="AX13" s="15"/>
+      <c r="AY13" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -1973,25 +1997,26 @@
       <c r="AP14" s="11" t="n">
         <v>28</v>
       </c>
-      <c r="AQ14" s="11" t="n">
+      <c r="AQ14" s="11"/>
+      <c r="AR14" s="11" t="n">
         <v>27</v>
       </c>
-      <c r="AR14" s="11"/>
       <c r="AS14" s="11"/>
       <c r="AT14" s="11"/>
       <c r="AU14" s="11"/>
       <c r="AV14" s="11"/>
       <c r="AW14" s="11"/>
-      <c r="AX14" s="10" t="s">
-        <v>70</v>
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="n">
@@ -2042,16 +2067,17 @@
       <c r="AU15" s="15"/>
       <c r="AV15" s="15"/>
       <c r="AW15" s="15"/>
-      <c r="AX15" s="14" t="s">
-        <v>72</v>
+      <c r="AX15" s="15"/>
+      <c r="AY15" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2108,16 +2134,17 @@
       <c r="AU16" s="11"/>
       <c r="AV16" s="11"/>
       <c r="AW16" s="11"/>
-      <c r="AX16" s="10" t="s">
-        <v>74</v>
+      <c r="AX16" s="11"/>
+      <c r="AY16" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -2168,16 +2195,17 @@
       <c r="AU17" s="15"/>
       <c r="AV17" s="15"/>
       <c r="AW17" s="15"/>
-      <c r="AX17" s="14" t="s">
-        <v>76</v>
+      <c r="AX17" s="15"/>
+      <c r="AY17" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2228,16 +2256,17 @@
       <c r="AU18" s="11"/>
       <c r="AV18" s="11"/>
       <c r="AW18" s="11"/>
-      <c r="AX18" s="10" t="s">
-        <v>78</v>
+      <c r="AX18" s="11"/>
+      <c r="AY18" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -2290,16 +2319,17 @@
       <c r="AU19" s="15"/>
       <c r="AV19" s="15"/>
       <c r="AW19" s="15"/>
-      <c r="AX19" s="14" t="s">
-        <v>80</v>
+      <c r="AX19" s="15"/>
+      <c r="AY19" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2352,16 +2382,17 @@
       <c r="AU20" s="11"/>
       <c r="AV20" s="11"/>
       <c r="AW20" s="11"/>
-      <c r="AX20" s="10" t="s">
-        <v>82</v>
+      <c r="AX20" s="11"/>
+      <c r="AY20" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -2412,16 +2443,17 @@
       <c r="AU21" s="15"/>
       <c r="AV21" s="15"/>
       <c r="AW21" s="15"/>
-      <c r="AX21" s="14" t="s">
-        <v>84</v>
+      <c r="AX21" s="15"/>
+      <c r="AY21" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2472,16 +2504,17 @@
       <c r="AU22" s="11"/>
       <c r="AV22" s="11"/>
       <c r="AW22" s="11"/>
-      <c r="AX22" s="10" t="s">
-        <v>86</v>
+      <c r="AX22" s="11"/>
+      <c r="AY22" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="23" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -2532,16 +2565,17 @@
       <c r="AU23" s="15"/>
       <c r="AV23" s="15"/>
       <c r="AW23" s="15"/>
-      <c r="AX23" s="14" t="s">
-        <v>88</v>
+      <c r="AX23" s="15"/>
+      <c r="AY23" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2592,16 +2626,17 @@
       <c r="AU24" s="11"/>
       <c r="AV24" s="11"/>
       <c r="AW24" s="11"/>
-      <c r="AX24" s="10" t="s">
-        <v>90</v>
+      <c r="AX24" s="11"/>
+      <c r="AY24" s="10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2657,23 +2692,26 @@
       <c r="AP25" s="15" t="n">
         <v>45</v>
       </c>
-      <c r="AQ25" s="15"/>
+      <c r="AQ25" s="15" t="n">
+        <v>44</v>
+      </c>
       <c r="AR25" s="15"/>
       <c r="AS25" s="15"/>
       <c r="AT25" s="15"/>
       <c r="AU25" s="15"/>
       <c r="AV25" s="15"/>
       <c r="AW25" s="15"/>
-      <c r="AX25" s="14" t="s">
-        <v>92</v>
+      <c r="AX25" s="15"/>
+      <c r="AY25" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2724,16 +2762,17 @@
       <c r="AU26" s="11"/>
       <c r="AV26" s="11"/>
       <c r="AW26" s="11"/>
-      <c r="AX26" s="10" t="s">
-        <v>94</v>
+      <c r="AX26" s="11"/>
+      <c r="AY26" s="10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -2784,16 +2823,17 @@
       <c r="AU27" s="15"/>
       <c r="AV27" s="15"/>
       <c r="AW27" s="15"/>
-      <c r="AX27" s="14" t="s">
-        <v>96</v>
+      <c r="AX27" s="15"/>
+      <c r="AY27" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -2848,16 +2888,17 @@
       <c r="AU28" s="11"/>
       <c r="AV28" s="11"/>
       <c r="AW28" s="11"/>
-      <c r="AX28" s="10" t="s">
-        <v>98</v>
+      <c r="AX28" s="11"/>
+      <c r="AY28" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2910,16 +2951,17 @@
       <c r="AU29" s="15"/>
       <c r="AV29" s="15"/>
       <c r="AW29" s="15"/>
-      <c r="AX29" s="14" t="s">
-        <v>100</v>
+      <c r="AX29" s="15"/>
+      <c r="AY29" s="14" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2970,16 +3012,17 @@
       <c r="AU30" s="11"/>
       <c r="AV30" s="11"/>
       <c r="AW30" s="11"/>
-      <c r="AX30" s="10" t="s">
-        <v>102</v>
+      <c r="AX30" s="11"/>
+      <c r="AY30" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -3034,16 +3077,17 @@
       <c r="AU31" s="15"/>
       <c r="AV31" s="15"/>
       <c r="AW31" s="15"/>
-      <c r="AX31" s="14" t="s">
-        <v>104</v>
+      <c r="AX31" s="15"/>
+      <c r="AY31" s="14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -3096,16 +3140,17 @@
       <c r="AU32" s="11"/>
       <c r="AV32" s="11"/>
       <c r="AW32" s="11"/>
-      <c r="AX32" s="10" t="s">
-        <v>106</v>
+      <c r="AX32" s="11"/>
+      <c r="AY32" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -3156,16 +3201,17 @@
       <c r="AU33" s="15"/>
       <c r="AV33" s="15"/>
       <c r="AW33" s="15"/>
-      <c r="AX33" s="14" t="s">
-        <v>108</v>
+      <c r="AX33" s="15"/>
+      <c r="AY33" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -3216,16 +3262,17 @@
       <c r="AU34" s="11"/>
       <c r="AV34" s="11"/>
       <c r="AW34" s="11"/>
-      <c r="AX34" s="10" t="s">
-        <v>110</v>
+      <c r="AX34" s="11"/>
+      <c r="AY34" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -3278,16 +3325,17 @@
       <c r="AU35" s="15"/>
       <c r="AV35" s="15"/>
       <c r="AW35" s="15"/>
-      <c r="AX35" s="14" t="s">
-        <v>112</v>
+      <c r="AX35" s="15"/>
+      <c r="AY35" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -3338,16 +3386,17 @@
       <c r="AU36" s="11"/>
       <c r="AV36" s="11"/>
       <c r="AW36" s="11"/>
-      <c r="AX36" s="10" t="s">
-        <v>114</v>
+      <c r="AX36" s="11"/>
+      <c r="AY36" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="37" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C37" s="15" t="n">
         <v>62</v>
@@ -3391,25 +3440,26 @@
       <c r="AN37" s="15"/>
       <c r="AO37" s="15"/>
       <c r="AP37" s="15"/>
-      <c r="AQ37" s="15" t="n">
+      <c r="AQ37" s="15"/>
+      <c r="AR37" s="15" t="n">
         <v>63</v>
       </c>
-      <c r="AR37" s="15"/>
       <c r="AS37" s="15"/>
       <c r="AT37" s="15"/>
       <c r="AU37" s="15"/>
       <c r="AV37" s="15"/>
       <c r="AW37" s="15"/>
-      <c r="AX37" s="14" t="s">
-        <v>116</v>
+      <c r="AX37" s="15"/>
+      <c r="AY37" s="14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -3462,16 +3512,17 @@
       <c r="AU38" s="11"/>
       <c r="AV38" s="11"/>
       <c r="AW38" s="11"/>
-      <c r="AX38" s="10" t="s">
-        <v>118</v>
+      <c r="AX38" s="11"/>
+      <c r="AY38" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="39" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
@@ -3524,16 +3575,17 @@
       <c r="AU39" s="15"/>
       <c r="AV39" s="15"/>
       <c r="AW39" s="15"/>
-      <c r="AX39" s="14" t="s">
-        <v>120</v>
+      <c r="AX39" s="15"/>
+      <c r="AY39" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -3575,181 +3627,185 @@
       <c r="AN40" s="11"/>
       <c r="AO40" s="11"/>
       <c r="AP40" s="11"/>
-      <c r="AQ40" s="11" t="n">
+      <c r="AQ40" s="11"/>
+      <c r="AR40" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="AR40" s="11" t="n">
+      <c r="AS40" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="AS40" s="11" t="n">
+      <c r="AT40" s="11" t="n">
         <v>70</v>
       </c>
-      <c r="AT40" s="11" t="n">
+      <c r="AU40" s="11" t="n">
         <v>71</v>
       </c>
-      <c r="AU40" s="11" t="n">
+      <c r="AV40" s="11" t="n">
         <v>72</v>
       </c>
-      <c r="AV40" s="11" t="n">
+      <c r="AW40" s="11" t="n">
         <v>73</v>
       </c>
-      <c r="AW40" s="11"/>
-      <c r="AX40" s="10" t="s">
-        <v>122</v>
+      <c r="AX40" s="11"/>
+      <c r="AY40" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z41" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH41" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ41" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK41" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ41" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR41" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU41" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV41" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW41" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX41" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY41" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T41" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="U41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W41" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y41" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB41" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD41" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE41" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF41" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG41" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI41" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ41" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM41" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN41" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ41" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR41" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT41" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU41" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV41" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW41" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX41" s="7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -3782,12 +3838,12 @@
       <c r="AF42" s="3"/>
       <c r="AG42" s="3"/>
       <c r="AH42" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI42" s="4"/>
       <c r="AJ42" s="4"/>
       <c r="AK42" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL42" s="5"/>
       <c r="AM42" s="5"/>
@@ -3800,7 +3856,8 @@
       <c r="AT42" s="5"/>
       <c r="AU42" s="5"/>
       <c r="AV42" s="5"/>
-      <c r="AW42" s="6"/>
+      <c r="AW42" s="5"/>
+      <c r="AX42" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3808,10 +3865,10 @@
     <mergeCell ref="I1:L2"/>
     <mergeCell ref="C4:AG4"/>
     <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AV4"/>
+    <mergeCell ref="AK4:AW4"/>
     <mergeCell ref="C42:AG42"/>
     <mergeCell ref="AH42:AJ42"/>
-    <mergeCell ref="AK42:AV42"/>
+    <mergeCell ref="AK42:AW42"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3849,1360 +3906,1360 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>131</v>
-      </c>
       <c r="G3" s="27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H3" s="27" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H4" s="27" t="n">
         <v>3</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="27" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>58</v>
       </c>
       <c r="H5" s="27" t="n">
         <v>4</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H6" s="27" t="n">
         <v>5</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="27" t="n">
         <v>6</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="27" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27" t="n">
         <v>8</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H10" s="27" t="n">
         <v>9</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H11" s="27" t="n">
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H12" s="27" t="n">
         <v>11</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H13" s="27" t="n">
         <v>12</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H14" s="27" t="n">
         <v>13</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27" t="n">
         <v>14</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>153</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>151</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27" t="n">
         <v>15</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27" t="n">
         <v>16</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27" t="n">
         <v>17</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="27" t="n">
         <v>18</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27" t="n">
         <v>19</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27" t="n">
         <v>20</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H22" s="27" t="n">
         <v>21</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27" t="n">
         <v>22</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H24" s="27" t="n">
         <v>23</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27" t="n">
         <v>24</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H26" s="27" t="n">
         <v>25</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H27" s="27" t="n">
         <v>26</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H28" s="27" t="n">
         <v>27</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H29" s="27" t="n">
         <v>28</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H30" s="27" t="n">
         <v>29</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H31" s="27" t="n">
         <v>30</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G32" s="27"/>
       <c r="H32" s="27" t="n">
         <v>31</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="27" t="n">
         <v>32</v>
       </c>
       <c r="I33" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="27" t="n">
         <v>33</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H35" s="27" t="n">
         <v>34</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H36" s="27" t="n">
         <v>35</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H37" s="27" t="n">
         <v>36</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G38" s="27"/>
       <c r="H38" s="27" t="n">
         <v>37</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H39" s="27" t="n">
         <v>38</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="27" t="n">
         <v>39</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H41" s="27" t="n">
         <v>40</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H42" s="27" t="n">
         <v>41</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H43" s="27" t="n">
         <v>42</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H44" s="27" t="n">
         <v>43</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H45" s="27" t="n">
         <v>44</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27" t="n">
         <v>45</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H47" s="27" t="n">
         <v>46</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F48" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H48" s="27" t="n">
         <v>47</v>
       </c>
       <c r="I48" s="27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G49" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H49" s="27" t="n">
         <v>48</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F50" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="27" t="n">
         <v>49</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F51" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H51" s="27" t="n">
         <v>50</v>
       </c>
       <c r="I51" s="27" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F52" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G52" s="27"/>
       <c r="H52" s="27" t="n">
         <v>51</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F53" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H53" s="27" t="n">
         <v>52</v>
       </c>
       <c r="I53" s="27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F54" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H54" s="27" t="n">
         <v>53</v>
       </c>
       <c r="I54" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F55" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G55" s="27"/>
       <c r="H55" s="27" t="n">
         <v>54</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G56" s="27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H56" s="27" t="n">
         <v>55</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F57" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27" t="n">
         <v>56</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F58" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H58" s="27" t="n">
         <v>57</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G59" s="27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H59" s="27" t="n">
         <v>58</v>
       </c>
       <c r="I59" s="27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F60" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G60" s="27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H60" s="27" t="n">
         <v>59</v>
       </c>
       <c r="I60" s="27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="27" t="n">
         <v>60</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H62" s="27" t="n">
         <v>61</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H63" s="27" t="n">
         <v>62</v>
       </c>
       <c r="I63" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="27" t="n">
         <v>63</v>
       </c>
       <c r="I64" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G65" s="27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H65" s="27" t="n">
         <v>64</v>
       </c>
       <c r="I65" s="27" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F66" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G66" s="27"/>
       <c r="H66" s="27" t="n">
         <v>65</v>
       </c>
       <c r="I66" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H67" s="27" t="n">
         <v>66</v>
       </c>
       <c r="I67" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G68" s="27"/>
       <c r="H68" s="27" t="n">
         <v>67</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G69" s="27" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H69" s="27" t="n">
         <v>68</v>
       </c>
       <c r="I69" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F70" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G70" s="27"/>
       <c r="H70" s="27" t="n">
         <v>69</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G71" s="27"/>
       <c r="H71" s="27" t="n">
         <v>70</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,19 +5268,19 @@
         <v>71</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F73" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G73" s="27"/>
       <c r="H73" s="27" t="n">
         <v>72</v>
       </c>
       <c r="I73" s="27" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5232,7 +5289,7 @@
         <v>73</v>
       </c>
       <c r="I74" s="27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add infinite do loop doc
</commit_message>
<xml_diff>
--- a/doc/parser/ll_table.xlsx
+++ b/doc/parser/ll_table.xlsx
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="190">
-  <si>
-    <t xml:space="preserve">LL Table IFJ17 (v1.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/11/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git q</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="191">
+  <si>
+    <t xml:space="preserve">LL Table IFJ17 (v1.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/11/2017</t>
   </si>
   <si>
     <t xml:space="preserve">Keywords</t>
@@ -347,52 +344,58 @@
     <t xml:space="preserve">27.</t>
   </si>
   <si>
-    <t xml:space="preserve">TestType</t>
+    <t xml:space="preserve">TestTypeStart</t>
   </si>
   <si>
     <t xml:space="preserve">28.</t>
   </si>
   <si>
+    <t xml:space="preserve">TestTypeEnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ExitStmt</t>
   </si>
   <si>
-    <t xml:space="preserve">29.</t>
+    <t xml:space="preserve">30.</t>
   </si>
   <si>
     <t xml:space="preserve">ContinueStmt</t>
   </si>
   <si>
-    <t xml:space="preserve">30.</t>
+    <t xml:space="preserve">31.</t>
   </si>
   <si>
     <t xml:space="preserve">LoopType</t>
   </si>
   <si>
-    <t xml:space="preserve">31.</t>
+    <t xml:space="preserve">32.</t>
   </si>
   <si>
     <t xml:space="preserve">ForStmt</t>
   </si>
   <si>
-    <t xml:space="preserve">32.</t>
+    <t xml:space="preserve">33.</t>
   </si>
   <si>
     <t xml:space="preserve">TypeOpt</t>
   </si>
   <si>
-    <t xml:space="preserve">33.</t>
+    <t xml:space="preserve">34.</t>
   </si>
   <si>
     <t xml:space="preserve">StepOpt</t>
   </si>
   <si>
-    <t xml:space="preserve">34.</t>
+    <t xml:space="preserve">35.</t>
   </si>
   <si>
     <t xml:space="preserve">IdOpt</t>
   </si>
   <si>
-    <t xml:space="preserve">35.</t>
+    <t xml:space="preserve">36.</t>
   </si>
   <si>
     <t xml:space="preserve">AssignOperator</t>
@@ -542,25 +545,25 @@
     <t xml:space="preserve">PRECEDENCNI ANALYZA</t>
   </si>
   <si>
+    <t xml:space="preserve">{ INTEGER }</t>
+  </si>
+  <si>
     <t xml:space="preserve">{ DO, FOR }</t>
   </si>
   <si>
-    <t xml:space="preserve">{ INTEGER }</t>
-  </si>
-  <si>
     <t xml:space="preserve">{ DOUBLE }</t>
   </si>
   <si>
+    <t xml:space="preserve">{ STRING }</t>
+  </si>
+  <si>
     <t xml:space="preserve">{ AS }</t>
   </si>
   <si>
-    <t xml:space="preserve">{ STRING }</t>
+    <t xml:space="preserve">{ BOOLEAN }</t>
   </si>
   <si>
     <t xml:space="preserve">{ STEP }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ BOOLEAN }</t>
   </si>
   <si>
     <t xml:space="preserve">{ =, -=. +=, *=, \=, /= }</t>
@@ -1081,10 +1084,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AY42"/>
+  <dimension ref="A1:AY43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1169,14 +1172,9 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1209,12 +1207,12 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL4" s="5"/>
       <c r="AM4" s="5"/>
@@ -1232,162 +1230,162 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AD5" s="3" t="s">
+      <c r="AE5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AG5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AH5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AK5" s="5" t="s">
+      <c r="AL5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AM5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AN5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AO5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AP5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AP5" s="5" t="s">
+      <c r="AQ5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AQ5" s="8" t="s">
+      <c r="AR5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AR5" s="8" t="s">
+      <c r="AS5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AS5" s="8" t="s">
+      <c r="AT5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AT5" s="8" t="s">
+      <c r="AU5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AU5" s="8" t="s">
+      <c r="AV5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AV5" s="8" t="s">
+      <c r="AW5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AW5" s="8" t="s">
+      <c r="AX5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AX5" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="AY5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="n">
@@ -1448,15 +1446,15 @@
       <c r="AW6" s="11"/>
       <c r="AX6" s="11"/>
       <c r="AY6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -1511,15 +1509,15 @@
         <v>3</v>
       </c>
       <c r="AY7" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="n">
@@ -1580,15 +1578,15 @@
       <c r="AW8" s="11"/>
       <c r="AX8" s="11"/>
       <c r="AY8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1665,15 +1663,15 @@
       <c r="AW9" s="15"/>
       <c r="AX9" s="15"/>
       <c r="AY9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1760,15 +1758,15 @@
       <c r="AW10" s="11"/>
       <c r="AX10" s="11"/>
       <c r="AY10" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>66</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1823,15 +1821,15 @@
       <c r="AW11" s="15"/>
       <c r="AX11" s="15"/>
       <c r="AY11" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1884,15 +1882,15 @@
       <c r="AW12" s="11"/>
       <c r="AX12" s="11"/>
       <c r="AY12" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1945,15 +1943,15 @@
       <c r="AW13" s="15"/>
       <c r="AX13" s="15"/>
       <c r="AY13" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2008,15 +2006,15 @@
       <c r="AW14" s="11"/>
       <c r="AX14" s="11"/>
       <c r="AY14" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>74</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="n">
@@ -2069,15 +2067,15 @@
       <c r="AW15" s="15"/>
       <c r="AX15" s="15"/>
       <c r="AY15" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2136,15 +2134,15 @@
       <c r="AW16" s="11"/>
       <c r="AX16" s="11"/>
       <c r="AY16" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>78</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -2197,15 +2195,15 @@
       <c r="AW17" s="15"/>
       <c r="AX17" s="15"/>
       <c r="AY17" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2258,15 +2256,15 @@
       <c r="AW18" s="11"/>
       <c r="AX18" s="11"/>
       <c r="AY18" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -2321,15 +2319,15 @@
       <c r="AW19" s="15"/>
       <c r="AX19" s="15"/>
       <c r="AY19" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2384,15 +2382,15 @@
       <c r="AW20" s="11"/>
       <c r="AX20" s="11"/>
       <c r="AY20" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>86</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -2445,15 +2443,15 @@
       <c r="AW21" s="15"/>
       <c r="AX21" s="15"/>
       <c r="AY21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2506,15 +2504,15 @@
       <c r="AW22" s="11"/>
       <c r="AX22" s="11"/>
       <c r="AY22" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>90</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -2567,15 +2565,15 @@
       <c r="AW23" s="15"/>
       <c r="AX23" s="15"/>
       <c r="AY23" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2628,15 +2626,15 @@
       <c r="AW24" s="11"/>
       <c r="AX24" s="11"/>
       <c r="AY24" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2703,15 +2701,15 @@
       <c r="AW25" s="15"/>
       <c r="AX25" s="15"/>
       <c r="AY25" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2764,15 +2762,15 @@
       <c r="AW26" s="11"/>
       <c r="AX26" s="11"/>
       <c r="AY26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>98</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -2825,15 +2823,15 @@
       <c r="AW27" s="15"/>
       <c r="AX27" s="15"/>
       <c r="AY27" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -2890,15 +2888,15 @@
       <c r="AW28" s="11"/>
       <c r="AX28" s="11"/>
       <c r="AY28" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>102</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2953,15 +2951,15 @@
       <c r="AW29" s="15"/>
       <c r="AX29" s="15"/>
       <c r="AY29" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>104</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -3014,15 +3012,15 @@
       <c r="AW30" s="11"/>
       <c r="AX30" s="11"/>
       <c r="AY30" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -3079,15 +3077,15 @@
       <c r="AW31" s="15"/>
       <c r="AX31" s="15"/>
       <c r="AY31" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -3142,15 +3140,15 @@
       <c r="AW32" s="11"/>
       <c r="AX32" s="11"/>
       <c r="AY32" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -3169,14 +3167,16 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
+      <c r="T33" s="15" t="n">
+        <v>57</v>
+      </c>
+      <c r="U33" s="15" t="n">
+        <v>58</v>
+      </c>
       <c r="V33" s="15"/>
       <c r="W33" s="15"/>
       <c r="X33" s="15"/>
-      <c r="Y33" s="15" t="n">
-        <v>57</v>
-      </c>
+      <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
       <c r="AA33" s="15"/>
       <c r="AB33" s="15"/>
@@ -3193,7 +3193,9 @@
       <c r="AM33" s="15"/>
       <c r="AN33" s="15"/>
       <c r="AO33" s="15"/>
-      <c r="AP33" s="15"/>
+      <c r="AP33" s="15" t="n">
+        <v>59</v>
+      </c>
       <c r="AQ33" s="15"/>
       <c r="AR33" s="15"/>
       <c r="AS33" s="15"/>
@@ -3203,15 +3205,15 @@
       <c r="AW33" s="15"/>
       <c r="AX33" s="15"/>
       <c r="AY33" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -3233,11 +3235,11 @@
       <c r="T34" s="11"/>
       <c r="U34" s="11"/>
       <c r="V34" s="11"/>
-      <c r="W34" s="11" t="n">
-        <v>58</v>
-      </c>
+      <c r="W34" s="11"/>
       <c r="X34" s="11"/>
-      <c r="Y34" s="11"/>
+      <c r="Y34" s="11" t="n">
+        <v>60</v>
+      </c>
       <c r="Z34" s="11"/>
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
@@ -3264,22 +3266,20 @@
       <c r="AW34" s="11"/>
       <c r="AX34" s="11"/>
       <c r="AY34" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="15" t="n">
-        <v>59</v>
-      </c>
+      <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
@@ -3296,13 +3296,13 @@
       <c r="T35" s="15"/>
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
+      <c r="W35" s="15" t="n">
+        <v>61</v>
+      </c>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
-      <c r="AA35" s="15" t="n">
-        <v>60</v>
-      </c>
+      <c r="AA35" s="15"/>
       <c r="AB35" s="15"/>
       <c r="AC35" s="15"/>
       <c r="AD35" s="15"/>
@@ -3327,20 +3327,22 @@
       <c r="AW35" s="15"/>
       <c r="AX35" s="15"/>
       <c r="AY35" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="n">
+        <v>62</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
@@ -3362,7 +3364,7 @@
       <c r="Y36" s="11"/>
       <c r="Z36" s="11"/>
       <c r="AA36" s="11" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB36" s="11"/>
       <c r="AC36" s="11"/>
@@ -3388,19 +3390,17 @@
       <c r="AW36" s="11"/>
       <c r="AX36" s="11"/>
       <c r="AY36" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" s="15" t="n">
-        <v>62</v>
-      </c>
+      <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -3424,7 +3424,9 @@
       <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
-      <c r="AA37" s="15"/>
+      <c r="AA37" s="15" t="n">
+        <v>64</v>
+      </c>
       <c r="AB37" s="15"/>
       <c r="AC37" s="15"/>
       <c r="AD37" s="15"/>
@@ -3441,9 +3443,7 @@
       <c r="AO37" s="15"/>
       <c r="AP37" s="15"/>
       <c r="AQ37" s="15"/>
-      <c r="AR37" s="15" t="n">
-        <v>63</v>
-      </c>
+      <c r="AR37" s="15"/>
       <c r="AS37" s="15"/>
       <c r="AT37" s="15"/>
       <c r="AU37" s="15"/>
@@ -3451,17 +3451,19 @@
       <c r="AW37" s="15"/>
       <c r="AX37" s="15"/>
       <c r="AY37" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="11" t="n">
+        <v>65</v>
+      </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -3491,9 +3493,7 @@
       <c r="AD38" s="11"/>
       <c r="AE38" s="11"/>
       <c r="AF38" s="11"/>
-      <c r="AG38" s="11" t="n">
-        <v>64</v>
-      </c>
+      <c r="AG38" s="11"/>
       <c r="AH38" s="11"/>
       <c r="AI38" s="11"/>
       <c r="AJ38" s="11"/>
@@ -3502,11 +3502,11 @@
       <c r="AM38" s="11"/>
       <c r="AN38" s="11"/>
       <c r="AO38" s="11"/>
-      <c r="AP38" s="11" t="n">
-        <v>65</v>
-      </c>
+      <c r="AP38" s="11"/>
       <c r="AQ38" s="11"/>
-      <c r="AR38" s="11"/>
+      <c r="AR38" s="11" t="n">
+        <v>66</v>
+      </c>
       <c r="AS38" s="11"/>
       <c r="AT38" s="11"/>
       <c r="AU38" s="11"/>
@@ -3514,15 +3514,15 @@
       <c r="AW38" s="11"/>
       <c r="AX38" s="11"/>
       <c r="AY38" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>122</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
@@ -3554,19 +3554,19 @@
       <c r="AD39" s="15"/>
       <c r="AE39" s="15"/>
       <c r="AF39" s="15"/>
-      <c r="AG39" s="15"/>
+      <c r="AG39" s="15" t="n">
+        <v>67</v>
+      </c>
       <c r="AH39" s="15"/>
       <c r="AI39" s="15"/>
       <c r="AJ39" s="15"/>
-      <c r="AK39" s="15" t="n">
-        <v>66</v>
-      </c>
+      <c r="AK39" s="15"/>
       <c r="AL39" s="15"/>
       <c r="AM39" s="15"/>
       <c r="AN39" s="15"/>
       <c r="AO39" s="15"/>
       <c r="AP39" s="15" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AQ39" s="15"/>
       <c r="AR39" s="15"/>
@@ -3577,15 +3577,15 @@
       <c r="AW39" s="15"/>
       <c r="AX39" s="15"/>
       <c r="AY39" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -3621,243 +3621,306 @@
       <c r="AH40" s="11"/>
       <c r="AI40" s="11"/>
       <c r="AJ40" s="11"/>
-      <c r="AK40" s="11"/>
+      <c r="AK40" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="AL40" s="11"/>
       <c r="AM40" s="11"/>
       <c r="AN40" s="11"/>
       <c r="AO40" s="11"/>
-      <c r="AP40" s="11"/>
+      <c r="AP40" s="11" t="n">
+        <v>70</v>
+      </c>
       <c r="AQ40" s="11"/>
-      <c r="AR40" s="11" t="n">
-        <v>68</v>
-      </c>
-      <c r="AS40" s="11" t="n">
-        <v>69</v>
-      </c>
-      <c r="AT40" s="11" t="n">
-        <v>70</v>
-      </c>
-      <c r="AU40" s="11" t="n">
-        <v>71</v>
-      </c>
-      <c r="AV40" s="11" t="n">
-        <v>72</v>
-      </c>
-      <c r="AW40" s="11" t="n">
-        <v>73</v>
-      </c>
+      <c r="AR40" s="11"/>
+      <c r="AS40" s="11"/>
+      <c r="AT40" s="11"/>
+      <c r="AU40" s="11"/>
+      <c r="AV40" s="11"/>
+      <c r="AW40" s="11"/>
       <c r="AX40" s="11"/>
       <c r="AY40" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="15"/>
+      <c r="AF41" s="15"/>
+      <c r="AG41" s="15"/>
+      <c r="AH41" s="15"/>
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="15"/>
+      <c r="AL41" s="15"/>
+      <c r="AM41" s="15"/>
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="15"/>
+      <c r="AQ41" s="15"/>
+      <c r="AR41" s="15" t="n">
+        <v>71</v>
+      </c>
+      <c r="AS41" s="15" t="n">
+        <v>72</v>
+      </c>
+      <c r="AT41" s="15" t="n">
+        <v>73</v>
+      </c>
+      <c r="AU41" s="15" t="n">
+        <v>74</v>
+      </c>
+      <c r="AV41" s="15" t="n">
+        <v>75</v>
+      </c>
+      <c r="AW41" s="15" t="n">
+        <v>76</v>
+      </c>
+      <c r="AX41" s="15"/>
+      <c r="AY41" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="K42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="L42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="M42" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="3" t="s">
+      <c r="N42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N41" s="3" t="s">
+      <c r="O42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O41" s="3" t="s">
+      <c r="P42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P41" s="3" t="s">
+      <c r="Q42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q41" s="3" t="s">
+      <c r="R42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R41" s="3" t="s">
+      <c r="S42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S41" s="3" t="s">
+      <c r="T42" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T41" s="3" t="s">
+      <c r="U42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U41" s="3" t="s">
+      <c r="V42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V41" s="3" t="s">
+      <c r="W42" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W41" s="3" t="s">
+      <c r="X42" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="X41" s="3" t="s">
+      <c r="Y42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Y41" s="3" t="s">
+      <c r="Z42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z41" s="3" t="s">
+      <c r="AA42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AA41" s="3" t="s">
+      <c r="AB42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AB41" s="3" t="s">
+      <c r="AC42" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AC41" s="3" t="s">
+      <c r="AD42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AD41" s="3" t="s">
+      <c r="AE42" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AE41" s="3" t="s">
+      <c r="AF42" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AF41" s="3" t="s">
+      <c r="AG42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AG41" s="3" t="s">
+      <c r="AH42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AH41" s="4" t="s">
+      <c r="AI42" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AI41" s="4" t="s">
+      <c r="AJ42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AJ41" s="4" t="s">
+      <c r="AK42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AK41" s="5" t="s">
+      <c r="AL42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AL41" s="5" t="s">
+      <c r="AM42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AM41" s="5" t="s">
+      <c r="AN42" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AN41" s="5" t="s">
+      <c r="AO42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AO41" s="5" t="s">
+      <c r="AP42" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AP41" s="5" t="s">
+      <c r="AQ42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AQ41" s="5" t="s">
+      <c r="AR42" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AR41" s="8" t="s">
+      <c r="AS42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AS41" s="8" t="s">
+      <c r="AT42" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AT41" s="8" t="s">
+      <c r="AU42" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AU41" s="8" t="s">
+      <c r="AV42" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AV41" s="8" t="s">
+      <c r="AW42" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AW41" s="8" t="s">
+      <c r="AX42" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AX41" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY41" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="3" t="s">
+      <c r="AY42" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="3"/>
+      <c r="AG43" s="3"/>
+      <c r="AH43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="3"/>
-      <c r="AG42" s="3"/>
-      <c r="AH42" s="4" t="s">
+      <c r="AI43" s="4"/>
+      <c r="AJ43" s="4"/>
+      <c r="AK43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AI42" s="4"/>
-      <c r="AJ42" s="4"/>
-      <c r="AK42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL42" s="5"/>
-      <c r="AM42" s="5"/>
-      <c r="AN42" s="5"/>
-      <c r="AO42" s="5"/>
-      <c r="AP42" s="5"/>
-      <c r="AQ42" s="5"/>
-      <c r="AR42" s="5"/>
-      <c r="AS42" s="5"/>
-      <c r="AT42" s="5"/>
-      <c r="AU42" s="5"/>
-      <c r="AV42" s="5"/>
-      <c r="AW42" s="5"/>
-      <c r="AX42" s="6"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="5"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="5"/>
+      <c r="AQ43" s="5"/>
+      <c r="AR43" s="5"/>
+      <c r="AS43" s="5"/>
+      <c r="AT43" s="5"/>
+      <c r="AU43" s="5"/>
+      <c r="AV43" s="5"/>
+      <c r="AW43" s="5"/>
+      <c r="AX43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3866,9 +3929,9 @@
     <mergeCell ref="C4:AG4"/>
     <mergeCell ref="AH4:AJ4"/>
     <mergeCell ref="AK4:AW4"/>
-    <mergeCell ref="C42:AG42"/>
-    <mergeCell ref="AH42:AJ42"/>
-    <mergeCell ref="AK42:AW42"/>
+    <mergeCell ref="C43:AG43"/>
+    <mergeCell ref="AH43:AJ43"/>
+    <mergeCell ref="AK43:AW43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3885,10 +3948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E87" activeCellId="0" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3906,766 +3969,766 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="27" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H4" s="27" t="n">
         <v>3</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="27" t="n">
         <v>4</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H6" s="27" t="n">
         <v>5</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="27" t="n">
         <v>6</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="27" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27" t="n">
         <v>8</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="27" t="n">
         <v>9</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H11" s="27" t="n">
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H12" s="27" t="n">
         <v>11</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>142</v>
-      </c>
       <c r="D13" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H13" s="27" t="n">
         <v>12</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H14" s="27" t="n">
         <v>13</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27" t="n">
         <v>14</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27" t="n">
         <v>15</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27" t="n">
         <v>16</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27" t="n">
         <v>17</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="27" t="n">
         <v>18</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27" t="n">
         <v>19</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27" t="n">
         <v>20</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="27" t="n">
         <v>21</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27" t="n">
         <v>22</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H24" s="27" t="n">
         <v>23</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27" t="n">
         <v>24</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H26" s="27" t="n">
         <v>25</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H27" s="27" t="n">
         <v>26</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" s="27" t="n">
         <v>27</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>143</v>
+        <v>109</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H29" s="27" t="n">
         <v>28</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>161</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H30" s="27" t="n">
         <v>29</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H31" s="27" t="n">
         <v>30</v>
@@ -4676,43 +4739,40 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G32" s="27"/>
       <c r="H32" s="27" t="n">
         <v>31</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>144</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="27" t="n">
@@ -4724,19 +4784,19 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>178</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="27" t="n">
@@ -4748,548 +4808,592 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H35" s="27" t="n">
         <v>34</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>143</v>
+        <v>123</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>172</v>
+        <v>133</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H36" s="27" t="n">
         <v>35</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>173</v>
+      </c>
       <c r="F37" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H37" s="27" t="n">
         <v>36</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G38" s="27"/>
       <c r="H38" s="27" t="n">
         <v>37</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="G39" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" s="27" t="n">
         <v>38</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="G40" s="27"/>
       <c r="H40" s="27" t="n">
         <v>39</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H41" s="27" t="n">
         <v>40</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H42" s="27" t="n">
         <v>41</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H43" s="27" t="n">
         <v>42</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H44" s="27" t="n">
         <v>43</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H45" s="27" t="n">
         <v>44</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27" t="n">
         <v>45</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H47" s="27" t="n">
         <v>46</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F48" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H48" s="27" t="n">
         <v>47</v>
       </c>
       <c r="I48" s="27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F49" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="G49" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H49" s="27" t="n">
         <v>48</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F50" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="G50" s="27"/>
       <c r="H50" s="27" t="n">
         <v>49</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F51" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H51" s="27" t="n">
         <v>50</v>
       </c>
       <c r="I51" s="27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F52" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G52" s="27"/>
       <c r="H52" s="27" t="n">
         <v>51</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F53" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H53" s="27" t="n">
         <v>52</v>
       </c>
       <c r="I53" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F54" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H54" s="27" t="n">
         <v>53</v>
       </c>
       <c r="I54" s="27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F55" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G55" s="27"/>
       <c r="H55" s="27" t="n">
         <v>54</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G56" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H56" s="27" t="n">
         <v>55</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F57" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27" t="n">
         <v>56</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F58" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H58" s="27" t="n">
         <v>57</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G59" s="27" t="s">
-        <v>112</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G59" s="27"/>
       <c r="H59" s="27" t="n">
         <v>58</v>
       </c>
       <c r="I59" s="27" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F60" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G60" s="27" t="s">
-        <v>114</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G60" s="27"/>
       <c r="H60" s="27" t="n">
         <v>59</v>
       </c>
       <c r="I60" s="27" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G61" s="27"/>
+        <v>133</v>
+      </c>
+      <c r="G61" s="27" t="s">
+        <v>111</v>
+      </c>
       <c r="H61" s="27" t="n">
         <v>60</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H62" s="27" t="n">
         <v>61</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H63" s="27" t="n">
         <v>62</v>
       </c>
       <c r="I63" s="27" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="27" t="n">
         <v>63</v>
       </c>
       <c r="I64" s="27" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G65" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H65" s="27" t="n">
         <v>64</v>
       </c>
       <c r="I65" s="27" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F66" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G66" s="27"/>
+        <v>133</v>
+      </c>
+      <c r="G66" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="H66" s="27" t="n">
         <v>65</v>
       </c>
       <c r="I66" s="27" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G67" s="27" t="s">
-        <v>122</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G67" s="27"/>
       <c r="H67" s="27" t="n">
         <v>66</v>
       </c>
       <c r="I67" s="27" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G68" s="27"/>
+        <v>133</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>121</v>
+      </c>
       <c r="H68" s="27" t="n">
         <v>67</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>124</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G69" s="27"/>
       <c r="H69" s="27" t="n">
         <v>68</v>
       </c>
       <c r="I69" s="27" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F70" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G70" s="27"/>
+        <v>133</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="H70" s="27" t="n">
         <v>69</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="0" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="G71" s="27"/>
       <c r="H71" s="27" t="n">
         <v>70</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G72" s="27"/>
+      <c r="F72" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>125</v>
+      </c>
       <c r="H72" s="27" t="n">
         <v>71</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F73" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="G73" s="27"/>
       <c r="H73" s="27" t="n">
         <v>72</v>
       </c>
       <c r="I73" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F74" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="G74" s="27"/>
       <c r="H74" s="27" t="n">
         <v>73</v>
       </c>
       <c r="I74" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="27"/>
+      <c r="H75" s="27" t="n">
+        <v>74</v>
+      </c>
+      <c r="I75" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="27"/>
+      <c r="H76" s="27" t="n">
+        <v>75</v>
+      </c>
+      <c r="I76" s="27" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G77" s="27"/>
+      <c r="H77" s="27" t="n">
+        <v>76</v>
+      </c>
+      <c r="I77" s="27" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>